<commit_message>
TODO + Klasse correctie
</commit_message>
<xml_diff>
--- a/Probleemstelling/Programma/Klassen.xlsx
+++ b/Probleemstelling/Programma/Klassen.xlsx
@@ -16,16 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>Boom</t>
-  </si>
-  <si>
-    <t>Grammatica</t>
-  </si>
-  <si>
-    <t>Symbool</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Terminal</t>
   </si>
@@ -63,14 +54,6 @@
     <t>Bedenking: Operand is ook een Non Terminal Nee?</t>
   </si>
   <si>
-    <t>PruneRegels</t>
-  </si>
-  <si>
-    <t>int levelCount
-Equation equation = E
-List&lt;List&lt;Equation&gt;&gt; lijstVanLevels</t>
-  </si>
-  <si>
     <t>Expand()</t>
   </si>
   <si>
@@ -84,9 +67,6 @@
   </si>
   <si>
     <t>Expand(Equation equation)</t>
-  </si>
-  <si>
-    <t>Tijd</t>
   </si>
   <si>
     <t>Input</t>
@@ -98,12 +78,6 @@
     <t>firstInputToTerminal()
 nextInputCheckSolutionSpace()
 evaluate()</t>
-  </si>
-  <si>
-    <t>Evalueer</t>
-  </si>
-  <si>
-    <t>Map&lt;String, Map&lt;Double, List&lt;String&gt;&gt;&gt; alreadyCalculated</t>
   </si>
   <si>
     <t>findSolution()
@@ -115,10 +89,6 @@
     <t xml:space="preserve">     evaluate()</t>
   </si>
   <si>
-    <t>expand(previousLevel)
-PruneRegels.prune(currentLevel)</t>
-  </si>
-  <si>
     <t>Start()
 TimeIsUp()</t>
   </si>
@@ -129,6 +99,45 @@
     <t>int inputCount
 List&lt;Equation&gt; solutionSpace
 File Boom</t>
+  </si>
+  <si>
+    <t>int levelCount
+Equation equation = E
+List&lt;List&lt;Equation&gt;&gt; lijstVanLevels (ArrayList)</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>List symbol</t>
+  </si>
+  <si>
+    <t>toString()</t>
+  </si>
+  <si>
+    <t>Map&lt;Equation, Map&lt;Double, List&lt;Equation&gt;&gt;&gt; alreadyCalculated</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>PruneRules</t>
+  </si>
+  <si>
+    <t>Grammar</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>expand(previousLevel)
+PruneRules.prune(currentLevel)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Evaluate</t>
   </si>
 </sst>
 </file>
@@ -174,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -398,11 +407,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -411,9 +457,102 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -438,9 +577,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -456,95 +592,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +687,7 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
@@ -808,7 +875,7 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
@@ -849,13 +916,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>598714</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>119743</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>598714</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>130628</xdr:rowOff>
@@ -896,13 +963,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>43543</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>174171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>587829</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>130629</xdr:rowOff>
@@ -943,13 +1010,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>65314</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>10886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>359229</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>141515</xdr:rowOff>
@@ -990,13 +1057,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>217714</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>10886</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>522514</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>163287</xdr:rowOff>
@@ -1037,13 +1104,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>413657</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>391886</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>141515</xdr:rowOff>
@@ -1084,13 +1151,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>500743</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>43543</xdr:rowOff>
@@ -1104,6 +1171,147 @@
         <a:xfrm flipV="1">
           <a:off x="5486400" y="2906486"/>
           <a:ext cx="5377543" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>174171</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>21771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>315686</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3831771" y="4212771"/>
+          <a:ext cx="1970315" cy="272143"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>544286</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3592286" y="1524000"/>
+          <a:ext cx="1219200" cy="1883229"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>32657</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119743</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>555171</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7347857" y="2786743"/>
+          <a:ext cx="4180114" cy="1012371"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1419,392 +1627,441 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X36"/>
+  <dimension ref="B1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3:S5"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="26" t="s">
+    <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="37"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="37"/>
+      <c r="X2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y2" s="10"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="12"/>
+      <c r="Q3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="12"/>
+      <c r="X3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="12"/>
+    </row>
+    <row r="4" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E4" s="30"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="28"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="14"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="34"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="34"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E6" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="Q6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="28"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E7" s="30"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="28"/>
+    </row>
+    <row r="8" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E8" s="13"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="14"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="10"/>
+      <c r="I12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="10"/>
+      <c r="P12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="10"/>
+      <c r="T12" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="36"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="37"/>
+    </row>
+    <row r="13" spans="2:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="12"/>
+      <c r="I13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="12"/>
+      <c r="P13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="12"/>
+      <c r="T13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="38"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="38"/>
+      <c r="X13" s="38"/>
+      <c r="Y13" s="38"/>
+      <c r="Z13" s="39"/>
+    </row>
+    <row r="14" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="30"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="28"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="14"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="42"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B15" s="30"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="28"/>
+      <c r="T15" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="45"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B16" s="30"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="T16" s="26"/>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="47"/>
+    </row>
+    <row r="17" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="30"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="14"/>
+      <c r="T17" s="26"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="46"/>
+      <c r="Z17" s="47"/>
+    </row>
+    <row r="18" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="30"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="T18" s="26"/>
+      <c r="U18" s="46"/>
+      <c r="V18" s="46"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="46"/>
+      <c r="Y18" s="46"/>
+      <c r="Z18" s="47"/>
+    </row>
+    <row r="19" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="I19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="10"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="49"/>
+      <c r="V19" s="49"/>
+      <c r="W19" s="49"/>
+      <c r="X19" s="49"/>
+      <c r="Y19" s="49"/>
+      <c r="Z19" s="50"/>
+    </row>
+    <row r="20" spans="2:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="57"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="I21" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="54"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="13"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="14"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="2:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="12"/>
+    </row>
+    <row r="27" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28"/>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E28" s="26"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
+    </row>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
+    </row>
+    <row r="30" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="13"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="14"/>
+    </row>
+    <row r="31" spans="2:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="E33" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="51"/>
+      <c r="I33" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="28"/>
-      <c r="V2" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="22"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="23"/>
-      <c r="P3" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="23"/>
-      <c r="V3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="W3" s="23"/>
-    </row>
-    <row r="4" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E4" s="31"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="30"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="25"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="36"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="36"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="30"/>
-      <c r="P6" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="30"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E7" s="31"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="29"/>
-      <c r="S7" s="30"/>
-    </row>
-    <row r="8" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="24"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="25"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="O10" t="s">
-        <v>29</v>
-      </c>
-      <c r="T10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="22"/>
-      <c r="H12" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="22"/>
-      <c r="O12" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="P12" s="22"/>
-      <c r="S12" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="28"/>
-    </row>
-    <row r="13" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="23"/>
-      <c r="H13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="23"/>
-      <c r="O13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13" s="23"/>
-      <c r="S13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="8"/>
-    </row>
-    <row r="14" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="31"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="25"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="11"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="31"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="S15" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="14"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B16" s="31"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="30"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="17"/>
-    </row>
-    <row r="17" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="31"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="25"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="17"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B18" s="31"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="17"/>
-    </row>
-    <row r="19" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="20"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="5"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-    </row>
-    <row r="24" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-    </row>
-    <row r="25" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="22"/>
-    </row>
-    <row r="26" spans="2:24" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="23"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E27" s="15"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E28" s="15"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="30"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="E29" s="15"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-    </row>
-    <row r="30" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E30" s="24"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="25"/>
-    </row>
-    <row r="31" spans="2:24" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="21" t="s">
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="E34" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="16"/>
+      <c r="G34" s="52"/>
+      <c r="I34" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="E33" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="22"/>
-      <c r="H33" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="41"/>
-      <c r="E34" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" s="41"/>
-      <c r="H34" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="I34" s="45"/>
-    </row>
-    <row r="35" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="42"/>
-      <c r="C35" s="43"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="H35" s="46"/>
-      <c r="I35" s="47"/>
-    </row>
-    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H36" s="48"/>
-      <c r="I36" s="49"/>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="52"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="22"/>
+    </row>
+    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I36" s="23"/>
+      <c r="J36" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="29">
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L22"/>
+    <mergeCell ref="T13:Z14"/>
+    <mergeCell ref="T15:Z19"/>
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="X3:Y4"/>
+    <mergeCell ref="T12:Z12"/>
+    <mergeCell ref="E6:I8"/>
+    <mergeCell ref="E3:I5"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="Q6:T8"/>
+    <mergeCell ref="E2:I2"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q14"/>
     <mergeCell ref="E34:F35"/>
     <mergeCell ref="B34:C35"/>
-    <mergeCell ref="H34:I36"/>
-    <mergeCell ref="E26:G30"/>
+    <mergeCell ref="I34:J36"/>
+    <mergeCell ref="E26:H30"/>
     <mergeCell ref="B13:D18"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E25:H25"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H13:K17"/>
-    <mergeCell ref="E6:H8"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="P3:S5"/>
-    <mergeCell ref="P6:S8"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="S13:X14"/>
-    <mergeCell ref="S15:X19"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="V3:W4"/>
-    <mergeCell ref="S12:X12"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L17"/>
+    <mergeCell ref="I19:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>